<commit_message>
Fixed branching and flushing It is functional but not pretty or elegant solution :) Had to hack the BEQ because we do pc update in MEM and we do MEM before Ex (minus 4) Can test by sending in jump1.txt in testcase folder Can use the list I've started in the excel sheet to add more testcases and to understand testcase assembler inputs and the testing explanation for each file
</commit_message>
<xml_diff>
--- a/testcases/Excel_project_testcases.xlsx
+++ b/testcases/Excel_project_testcases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozgul Zeki\Desktop\jsarmstr\FromWorkLaptop_Jess_March2021\jsarmstr\PSU\21S_Classes\ECE586\Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozgul Zeki\PSU586_FinalProject\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A61EFD2-EC94-4ACC-808C-94B33107A52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47600E02-5B92-45C0-9E21-5DF112313D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="2415" windowWidth="18000" windowHeight="9480" xr2:uid="{D50AE810-5038-48AF-9E4E-5572CA928CD4}"/>
+    <workbookView xWindow="5625" yWindow="2415" windowWidth="18000" windowHeight="9480" activeTab="1" xr2:uid="{D50AE810-5038-48AF-9E4E-5572CA928CD4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="decode" sheetId="1" r:id="rId1"/>
+    <sheet name="test_case_summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>opcode</t>
   </si>
@@ -58,6 +59,41 @@
   </si>
   <si>
     <t>hex</t>
+  </si>
+  <si>
+    <t>Feature to test</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Assembler input</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>jumpPostAddi</t>
+  </si>
+  <si>
+    <t>W/O Forwarding
+Passing/Not</t>
+  </si>
+  <si>
+    <t>W/ Forwarding
+Passing/Not</t>
+  </si>
+  <si>
+    <t>jump1.txt</t>
+  </si>
+  <si>
+    <t>Input file</t>
+  </si>
+  <si>
+    <t>Passing</t>
+  </si>
+  <si>
+    <t>branching and flushing</t>
   </si>
 </sst>
 </file>
@@ -73,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +128,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -105,8 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -116,10 +162,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC965A3A-B529-4CD1-A97D-8C1150E0050A}">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AI19" sqref="AI19"/>
     </sheetView>
   </sheetViews>
@@ -546,130 +592,130 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
         <v>3</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="2">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3">
         <v>32</v>
       </c>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
       <c r="AG4" t="s">
         <v>6</v>
       </c>
@@ -782,54 +828,54 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
         <v>4</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3">
         <v>3</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3">
         <v>8</v>
       </c>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
       <c r="AG6" t="s">
         <v>6</v>
       </c>
@@ -842,50 +888,50 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="1">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3">
         <v>4</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3">
         <v>9</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1">
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3">
         <v>32</v>
       </c>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
       <c r="AG7" t="s">
         <v>7</v>
       </c>
@@ -998,54 +1044,54 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
         <v>2</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3">
         <v>4</v>
       </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3">
         <v>4</v>
       </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1">
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3">
         <v>8</v>
       </c>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
       <c r="AG9" t="s">
         <v>7</v>
       </c>
@@ -1057,52 +1103,52 @@
         <v>00244810</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1">
+      <c r="A11" s="3">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
         <v>2</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3">
         <v>3</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="2">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="1">
-        <v>0</v>
-      </c>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3">
         <v>32</v>
       </c>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
       <c r="AG11" t="s">
         <v>6</v>
       </c>
@@ -1215,62 +1261,62 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
+      <c r="A13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(A12,B12,C12,D12))</f>
         <v>0</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="str">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(E12,F12,G12,H12))</f>
         <v>0</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="str">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(I12,J12,K12,L12))</f>
         <v>4</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1" t="str">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(M12,N12,O12,P12))</f>
         <v>3</v>
       </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1" t="str">
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Q12,R12,S12,T12))</f>
         <v>0</v>
       </c>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1" t="str">
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(U12,V12,W12,X12))</f>
         <v>8</v>
       </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1" t="str">
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Y12,Z12,AA12,AB12))</f>
         <v>1</v>
       </c>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1" t="str">
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(AC12,AD12,AE12,AF12))</f>
         <v>0</v>
       </c>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
       <c r="AG13" t="s">
         <v>6</v>
       </c>
@@ -1283,50 +1329,50 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="3">
+      <c r="A14" s="3">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5">
         <v>5</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="1">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3">
         <v>4</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3">
         <v>9</v>
       </c>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1">
-        <v>0</v>
-      </c>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1">
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3">
+        <v>0</v>
+      </c>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3">
         <v>32</v>
       </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
       <c r="AG14" t="s">
         <v>7</v>
       </c>
@@ -1436,62 +1482,62 @@
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
+      <c r="A16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(A15,B15,C15,D15))</f>
         <v>0</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="str">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(E15,F15,G15,H15))</f>
         <v>0</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="str">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(I15,J15,K15,L15))</f>
         <v>A</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1" t="str">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(M15,N15,O15,P15))</f>
         <v>4</v>
       </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1" t="str">
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Q15,R15,S15,T15))</f>
         <v>4</v>
       </c>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1" t="str">
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(U15,V15,W15,X15))</f>
         <v>8</v>
       </c>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1" t="str">
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Y15,Z15,AA15,AB15))</f>
         <v>1</v>
       </c>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1" t="str">
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(AC15,AD15,AE15,AF15))</f>
         <v>0</v>
       </c>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
       <c r="AG16" t="s">
         <v>7</v>
       </c>
@@ -1504,50 +1550,50 @@
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="1">
+      <c r="A17" s="3">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="3">
         <v>3</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="3">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="5">
         <v>6</v>
       </c>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="1">
-        <v>0</v>
-      </c>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1">
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3">
         <v>32</v>
       </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
       <c r="AG17" t="s">
         <v>6</v>
       </c>
@@ -1660,62 +1706,62 @@
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
+      <c r="A19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(A18,B18,C18,D18))</f>
         <v>0</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="str">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(E18,F18,G18,H18))</f>
         <v>0</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1" t="str">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(I18,J18,K18,L18))</f>
         <v>2</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1" t="str">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(M18,N18,O18,P18))</f>
         <v>3</v>
       </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1" t="str">
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Q18,R18,S18,T18))</f>
         <v>3</v>
       </c>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1" t="str">
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(U18,V18,W18,X18))</f>
         <v>0</v>
       </c>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1" t="str">
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(Y18,Z18,AA18,AB18))</f>
         <v>1</v>
       </c>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1" t="str">
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3" t="str">
         <f>BIN2HEX(CONCATENATE(AC18,AD18,AE18,AF18))</f>
         <v>0</v>
       </c>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
       <c r="AH19" t="s">
         <v>10</v>
       </c>
@@ -1726,48 +1772,24 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="Y19:AB19"/>
-    <mergeCell ref="AC19:AF19"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="Q19:T19"/>
-    <mergeCell ref="U19:X19"/>
-    <mergeCell ref="Y16:AB16"/>
-    <mergeCell ref="AC16:AF16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="V17:Z17"/>
-    <mergeCell ref="AA17:AF17"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="AC13:AF13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="V14:Z14"/>
-    <mergeCell ref="AA14:AF14"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="U13:X13"/>
-    <mergeCell ref="AA11:AF11"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="V11:Z11"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="AA7:AF7"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="V4:Z4"/>
+    <mergeCell ref="AA4:AF4"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="V7:Z7"/>
     <mergeCell ref="Y6:AB6"/>
     <mergeCell ref="AC6:AF6"/>
     <mergeCell ref="A9:D9"/>
@@ -1784,25 +1806,110 @@
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="U6:X6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:Z7"/>
-    <mergeCell ref="AA7:AF7"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="V4:Z4"/>
-    <mergeCell ref="AA4:AF4"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="AA11:AF11"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="V11:Z11"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="AC13:AF13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="V14:Z14"/>
+    <mergeCell ref="AA14:AF14"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="Y16:AB16"/>
+    <mergeCell ref="AC16:AF16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="V17:Z17"/>
+    <mergeCell ref="AA17:AF17"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q16:T16"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="Y19:AB19"/>
+    <mergeCell ref="AC19:AF19"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="Q19:T19"/>
+    <mergeCell ref="U19:X19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434BF61-29AD-4769-9A7A-822F44B5AD13}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding some testcases to use for quick regression checks to make sure we aren't breaking as we go along
</commit_message>
<xml_diff>
--- a/testcases/Excel_project_testcases.xlsx
+++ b/testcases/Excel_project_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozgul Zeki\PSU586_FinalProject\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47600E02-5B92-45C0-9E21-5DF112313D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE93E5-C98D-41CF-8029-F0350947B9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5625" yWindow="2415" windowWidth="18000" windowHeight="9480" activeTab="1" xr2:uid="{D50AE810-5038-48AF-9E4E-5572CA928CD4}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>opcode</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>BEQ</t>
-  </si>
-  <si>
-    <t>jumpPostAddi</t>
   </si>
   <si>
     <t>W/O Forwarding
@@ -94,6 +91,61 @@
   </si>
   <si>
     <t>branching and flushing</t>
+  </si>
+  <si>
+    <t>Expected output:</t>
+  </si>
+  <si>
+    <t>Skip R5-R7,
+Jump forward by 4 lines,
+R9 should be first reg listed</t>
+  </si>
+  <si>
+    <t>jumpPostAddi_1.txt</t>
+  </si>
+  <si>
+    <t>jumpPostAddi_4.txt</t>
+  </si>
+  <si>
+    <t>jump2.txt</t>
+  </si>
+  <si>
+    <t>Skip R5,
+Jump forward by 1 line,
+R6 should be first reg listed</t>
+  </si>
+  <si>
+    <t>Copy/paste to run</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ./sim -i testcases/jump2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ./sim -i testcases/jump1.txt</t>
+  </si>
+  <si>
+    <t>ADDI</t>
+  </si>
+  <si>
+    <t>add immediates</t>
+  </si>
+  <si>
+    <t>R6-R14 values in order: 3, 4, 5, 6, 7, 8, 9, 10, 11</t>
+  </si>
+  <si>
+    <t>Read after Write</t>
+  </si>
+  <si>
+    <t>sequential read after right (hazard with EX)</t>
+  </si>
+  <si>
+    <t>rawEX_1.txt</t>
+  </si>
+  <si>
+    <t>raw1.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ./sim -i testcases/raw1.txt</t>
   </si>
 </sst>
 </file>
@@ -109,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +186,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -147,12 +205,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -162,10 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,50 +651,50 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3" t="s">
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -672,50 +731,50 @@
       <c r="AF3" s="2"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5">
         <v>3</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3">
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5">
         <v>32</v>
       </c>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
       <c r="AG4" t="s">
         <v>6</v>
       </c>
@@ -828,54 +887,54 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3">
+      <c r="A6" s="5">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5">
         <v>4</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5">
         <v>3</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5">
         <v>8</v>
       </c>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
       <c r="AG6" t="s">
         <v>6</v>
       </c>
@@ -888,50 +947,50 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="3">
+      <c r="A7" s="5">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5">
         <v>4</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5">
         <v>9</v>
       </c>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3">
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5">
         <v>32</v>
       </c>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
       <c r="AG7" t="s">
         <v>7</v>
       </c>
@@ -1044,54 +1103,54 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3">
+      <c r="A9" s="5">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5">
         <v>2</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5">
         <v>4</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5">
         <v>4</v>
       </c>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3">
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5">
         <v>8</v>
       </c>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
       <c r="AG9" t="s">
         <v>7</v>
       </c>
@@ -1105,50 +1164,50 @@
     </row>
     <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3">
+      <c r="A11" s="5">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>2</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5">
         <v>3</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="4">
-        <v>1</v>
-      </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="3">
-        <v>0</v>
-      </c>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3">
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="5">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5">
         <v>32</v>
       </c>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
       <c r="AG11" t="s">
         <v>6</v>
       </c>
@@ -1261,62 +1320,62 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(A12,B12,C12,D12))</f>
         <v>0</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="str">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(E12,F12,G12,H12))</f>
         <v>0</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="str">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(I12,J12,K12,L12))</f>
         <v>4</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3" t="str">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(M12,N12,O12,P12))</f>
         <v>3</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3" t="str">
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Q12,R12,S12,T12))</f>
         <v>0</v>
       </c>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3" t="str">
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(U12,V12,W12,X12))</f>
         <v>8</v>
       </c>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3" t="str">
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Y12,Z12,AA12,AB12))</f>
         <v>1</v>
       </c>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3" t="str">
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(AC12,AD12,AE12,AF12))</f>
         <v>0</v>
       </c>
-      <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
       <c r="AG13" t="s">
         <v>6</v>
       </c>
@@ -1329,50 +1388,50 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5">
+      <c r="A14" s="5">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7">
         <v>5</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="3">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="5">
         <v>4</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5">
         <v>9</v>
       </c>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3">
-        <v>0</v>
-      </c>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3">
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5">
         <v>32</v>
       </c>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
       <c r="AG14" t="s">
         <v>7</v>
       </c>
@@ -1482,62 +1541,62 @@
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="str">
+      <c r="A16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(A15,B15,C15,D15))</f>
         <v>0</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="str">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(E15,F15,G15,H15))</f>
         <v>0</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="str">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(I15,J15,K15,L15))</f>
         <v>A</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3" t="str">
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(M15,N15,O15,P15))</f>
         <v>4</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3" t="str">
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Q15,R15,S15,T15))</f>
         <v>4</v>
       </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3" t="str">
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(U15,V15,W15,X15))</f>
         <v>8</v>
       </c>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3" t="str">
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Y15,Z15,AA15,AB15))</f>
         <v>1</v>
       </c>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3" t="str">
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(AC15,AD15,AE15,AF15))</f>
         <v>0</v>
       </c>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
       <c r="AG16" t="s">
         <v>7</v>
       </c>
@@ -1550,50 +1609,50 @@
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>0</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="3">
+      <c r="A17" s="5">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5">
         <v>3</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="5">
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="7">
         <v>6</v>
       </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="3">
-        <v>0</v>
-      </c>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3">
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5">
         <v>32</v>
       </c>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
       <c r="AG17" t="s">
         <v>6</v>
       </c>
@@ -1706,62 +1765,62 @@
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="str">
+      <c r="A19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(A18,B18,C18,D18))</f>
         <v>0</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="str">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(E18,F18,G18,H18))</f>
         <v>0</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="str">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(I18,J18,K18,L18))</f>
         <v>2</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3" t="str">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(M18,N18,O18,P18))</f>
         <v>3</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3" t="str">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Q18,R18,S18,T18))</f>
         <v>3</v>
       </c>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3" t="str">
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(U18,V18,W18,X18))</f>
         <v>0</v>
       </c>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3" t="str">
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(Y18,Z18,AA18,AB18))</f>
         <v>1</v>
       </c>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3" t="str">
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5" t="str">
         <f>BIN2HEX(CONCATENATE(AC18,AD18,AE18,AF18))</f>
         <v>0</v>
       </c>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
       <c r="AH19" t="s">
         <v>10</v>
       </c>
@@ -1772,12 +1831,62 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="Y19:AB19"/>
+    <mergeCell ref="AC19:AF19"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="Q19:T19"/>
+    <mergeCell ref="U19:X19"/>
+    <mergeCell ref="Y16:AB16"/>
+    <mergeCell ref="AC16:AF16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="V17:Z17"/>
+    <mergeCell ref="AA17:AF17"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q16:T16"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="AC13:AF13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="V14:Z14"/>
+    <mergeCell ref="AA14:AF14"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="AA11:AF11"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="V11:Z11"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="AC9:AF9"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="Q9:T9"/>
     <mergeCell ref="AA7:AF7"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="G4:K4"/>
@@ -1792,62 +1901,12 @@
     <mergeCell ref="V7:Z7"/>
     <mergeCell ref="Y6:AB6"/>
     <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="U9:X9"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="AC9:AF9"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="AA11:AF11"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="V11:Z11"/>
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="AC13:AF13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="V14:Z14"/>
-    <mergeCell ref="AA14:AF14"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="U13:X13"/>
-    <mergeCell ref="Y16:AB16"/>
-    <mergeCell ref="AC16:AF16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="V17:Z17"/>
-    <mergeCell ref="AA17:AF17"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="Y19:AB19"/>
-    <mergeCell ref="AC19:AF19"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="Q19:T19"/>
-    <mergeCell ref="U19:X19"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1855,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434BF61-29AD-4769-9A7A-822F44B5AD13}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,21 +1925,21 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1889,24 +1948,124 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>